<commit_message>
Task 1, 2 and 3 were finished
Task 1, 2 and 3 were finished
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CapoBizkitz\Documents\Leander_Pace_SWD63A_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CapoBizkitz\Documents\GitHub\Leander_Pace_SWD63A_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD51697-DDA5-4481-88C5-44B91FBA9A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8390118-6810-42CB-8FBC-9B97FD8D5030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="4215" windowWidth="24885" windowHeight="11385" activeTab="1" xr2:uid="{CC92C735-8AF0-4F0A-B2CB-5E9019629F5E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CC92C735-8AF0-4F0A-B2CB-5E9019629F5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected" sheetId="1" r:id="rId1"/>
@@ -3746,7 +3746,7 @@
   <dimension ref="A1:AY44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="AN19" sqref="AN19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4923,7 +4923,7 @@
       <c r="AM18" s="9"/>
       <c r="AN18" s="9"/>
       <c r="AO18" s="9"/>
-      <c r="AP18" s="10"/>
+      <c r="AP18" s="9"/>
       <c r="AQ18" s="9"/>
       <c r="AR18" s="9"/>
       <c r="AS18" s="9"/>
@@ -4971,14 +4971,14 @@
       <c r="AF19" s="9"/>
       <c r="AG19" s="9"/>
       <c r="AH19" s="9"/>
-      <c r="AI19" s="10"/>
-      <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
       <c r="AL19" s="10"/>
       <c r="AM19" s="10"/>
-      <c r="AN19" s="10"/>
-      <c r="AO19" s="10"/>
-      <c r="AP19" s="10"/>
+      <c r="AN19" s="9"/>
+      <c r="AO19" s="9"/>
+      <c r="AP19" s="9"/>
       <c r="AQ19" s="9"/>
       <c r="AR19" s="9"/>
       <c r="AS19" s="9"/>
@@ -5032,8 +5032,8 @@
       <c r="AL20" s="9"/>
       <c r="AM20" s="9"/>
       <c r="AN20" s="9"/>
-      <c r="AO20" s="10"/>
-      <c r="AP20" s="10"/>
+      <c r="AO20" s="9"/>
+      <c r="AP20" s="9"/>
       <c r="AQ20" s="9"/>
       <c r="AR20" s="9"/>
       <c r="AS20" s="9"/>
@@ -5195,10 +5195,10 @@
       <c r="AJ23" s="9"/>
       <c r="AK23" s="13"/>
       <c r="AL23" s="13"/>
-      <c r="AM23" s="9"/>
+      <c r="AM23" s="13"/>
       <c r="AN23" s="9"/>
-      <c r="AO23" s="1"/>
-      <c r="AP23" s="1"/>
+      <c r="AO23" s="9"/>
+      <c r="AP23" s="9"/>
       <c r="AQ23" s="9"/>
       <c r="AR23" s="9"/>
       <c r="AS23" s="9"/>
@@ -5249,10 +5249,10 @@
       <c r="AI24" s="9"/>
       <c r="AJ24" s="9"/>
       <c r="AK24" s="9"/>
-      <c r="AM24" s="13"/>
-      <c r="AN24" s="13"/>
-      <c r="AO24" s="1"/>
-      <c r="AP24" s="1"/>
+      <c r="AM24" s="9"/>
+      <c r="AN24" s="9"/>
+      <c r="AO24" s="9"/>
+      <c r="AP24" s="9"/>
       <c r="AQ24" s="9"/>
       <c r="AR24" s="9"/>
       <c r="AS24" s="9"/>
@@ -5306,10 +5306,10 @@
       <c r="AL25" s="9"/>
       <c r="AM25" s="9"/>
       <c r="AN25" s="9"/>
-      <c r="AO25" s="13"/>
+      <c r="AO25" s="9"/>
       <c r="AP25" s="9"/>
-      <c r="AQ25" s="1"/>
-      <c r="AR25" s="1"/>
+      <c r="AQ25" s="9"/>
+      <c r="AR25" s="9"/>
       <c r="AS25" s="9"/>
       <c r="AT25" s="9"/>
       <c r="AU25" s="9"/>
@@ -5361,10 +5361,10 @@
       <c r="AL26" s="9"/>
       <c r="AM26" s="9"/>
       <c r="AN26" s="9"/>
-      <c r="AO26" s="13"/>
-      <c r="AP26" s="13"/>
-      <c r="AQ26" s="13"/>
-      <c r="AR26" s="1"/>
+      <c r="AO26" s="9"/>
+      <c r="AP26" s="9"/>
+      <c r="AQ26" s="9"/>
+      <c r="AR26" s="9"/>
       <c r="AS26" s="9"/>
       <c r="AT26" s="9"/>
       <c r="AU26" s="9"/>
@@ -5418,8 +5418,8 @@
       <c r="AN27" s="9"/>
       <c r="AO27" s="9"/>
       <c r="AP27" s="9"/>
-      <c r="AQ27" s="13"/>
-      <c r="AR27" s="1"/>
+      <c r="AQ27" s="9"/>
+      <c r="AR27" s="9"/>
       <c r="AS27" s="9"/>
       <c r="AT27" s="9"/>
       <c r="AU27" s="9"/>
@@ -5473,8 +5473,8 @@
       <c r="AN28" s="9"/>
       <c r="AO28" s="9"/>
       <c r="AP28" s="9"/>
-      <c r="AQ28" s="13"/>
-      <c r="AR28" s="13"/>
+      <c r="AQ28" s="9"/>
+      <c r="AR28" s="9"/>
       <c r="AS28" s="9"/>
       <c r="AT28" s="9"/>
       <c r="AU28" s="9"/>
@@ -5527,9 +5527,9 @@
       <c r="AM29" s="9"/>
       <c r="AN29" s="9"/>
       <c r="AO29" s="9"/>
-      <c r="AP29" s="13"/>
-      <c r="AQ29" s="13"/>
-      <c r="AR29" s="13"/>
+      <c r="AP29" s="9"/>
+      <c r="AQ29" s="9"/>
+      <c r="AR29" s="9"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
       <c r="AU29" s="9"/>
@@ -5638,9 +5638,9 @@
       <c r="AN31" s="9"/>
       <c r="AO31" s="9"/>
       <c r="AP31" s="9"/>
-      <c r="AQ31" s="24"/>
-      <c r="AR31" s="24"/>
-      <c r="AS31" s="24"/>
+      <c r="AQ31" s="9"/>
+      <c r="AR31" s="9"/>
+      <c r="AS31" s="9"/>
       <c r="AT31" s="9"/>
       <c r="AU31" s="9"/>
       <c r="AV31" s="9"/>
@@ -5693,10 +5693,10 @@
       <c r="AN32" s="9"/>
       <c r="AO32" s="9"/>
       <c r="AP32" s="9"/>
-      <c r="AQ32" s="1"/>
+      <c r="AQ32" s="9"/>
       <c r="AR32" s="9"/>
-      <c r="AS32" s="24"/>
-      <c r="AT32" s="24"/>
+      <c r="AS32" s="9"/>
+      <c r="AT32" s="9"/>
       <c r="AU32" s="9"/>
       <c r="AV32" s="9"/>
       <c r="AW32" s="9"/>
@@ -5748,11 +5748,11 @@
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
       <c r="AP33" s="9"/>
-      <c r="AQ33" s="1"/>
+      <c r="AQ33" s="9"/>
       <c r="AR33" s="9"/>
       <c r="AS33" s="9"/>
-      <c r="AT33" s="24"/>
-      <c r="AU33" s="24"/>
+      <c r="AT33" s="9"/>
+      <c r="AU33" s="9"/>
       <c r="AV33" s="9"/>
       <c r="AW33" s="9"/>
       <c r="AX33" s="9"/>
@@ -5861,8 +5861,8 @@
       <c r="AR35" s="9"/>
       <c r="AS35" s="9"/>
       <c r="AT35" s="9"/>
-      <c r="AU35" s="26"/>
-      <c r="AV35" s="25"/>
+      <c r="AU35" s="9"/>
+      <c r="AV35" s="9"/>
       <c r="AW35" s="9"/>
       <c r="AX35" s="9"/>
       <c r="AY35" s="9"/>
@@ -5916,8 +5916,8 @@
       <c r="AR36" s="9"/>
       <c r="AS36" s="9"/>
       <c r="AT36" s="9"/>
-      <c r="AU36" s="25"/>
-      <c r="AV36" s="25"/>
+      <c r="AU36" s="9"/>
+      <c r="AV36" s="9"/>
       <c r="AW36" s="9"/>
       <c r="AX36" s="9"/>
       <c r="AY36" s="9"/>
@@ -5973,7 +5973,7 @@
       <c r="AT37" s="9"/>
       <c r="AU37" s="9"/>
       <c r="AV37" s="9"/>
-      <c r="AW37" s="25"/>
+      <c r="AW37" s="9"/>
       <c r="AX37" s="9"/>
       <c r="AY37" s="9"/>
     </row>
@@ -6027,7 +6027,7 @@
       <c r="AS38" s="9"/>
       <c r="AT38" s="9"/>
       <c r="AU38" s="9"/>
-      <c r="AV38" s="25"/>
+      <c r="AV38" s="9"/>
       <c r="AW38" s="9"/>
       <c r="AX38" s="9"/>
       <c r="AY38" s="9"/>
@@ -6083,7 +6083,8 @@
       <c r="AT39" s="9"/>
       <c r="AU39" s="9"/>
       <c r="AV39" s="9"/>
-      <c r="AX39" s="25"/>
+      <c r="AW39" s="9"/>
+      <c r="AX39" s="9"/>
       <c r="AY39" s="9"/>
     </row>
     <row r="40" spans="1:51" ht="45" x14ac:dyDescent="0.25">
@@ -6188,10 +6189,10 @@
       <c r="AP41" s="9"/>
       <c r="AQ41" s="9"/>
       <c r="AR41" s="9"/>
-      <c r="AS41" s="1"/>
-      <c r="AT41" s="1"/>
-      <c r="AU41" s="27"/>
-      <c r="AV41" s="27"/>
+      <c r="AS41" s="9"/>
+      <c r="AT41" s="9"/>
+      <c r="AU41" s="9"/>
+      <c r="AV41" s="9"/>
       <c r="AW41" s="9"/>
       <c r="AX41" s="9"/>
       <c r="AY41" s="9"/>
@@ -6243,12 +6244,12 @@
       <c r="AP42" s="9"/>
       <c r="AQ42" s="9"/>
       <c r="AR42" s="9"/>
-      <c r="AS42" s="1"/>
-      <c r="AT42" s="1"/>
+      <c r="AS42" s="9"/>
+      <c r="AT42" s="9"/>
       <c r="AU42" s="9"/>
       <c r="AV42" s="9"/>
-      <c r="AW42" s="27"/>
-      <c r="AX42" s="27"/>
+      <c r="AW42" s="9"/>
+      <c r="AX42" s="9"/>
       <c r="AY42" s="9"/>
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.25">
@@ -6298,13 +6299,13 @@
       <c r="AP43" s="9"/>
       <c r="AQ43" s="9"/>
       <c r="AR43" s="9"/>
-      <c r="AS43" s="1"/>
-      <c r="AT43" s="1"/>
+      <c r="AS43" s="9"/>
+      <c r="AT43" s="9"/>
       <c r="AU43" s="9"/>
       <c r="AV43" s="9"/>
       <c r="AW43" s="9"/>
       <c r="AX43" s="9"/>
-      <c r="AY43" s="27"/>
+      <c r="AY43" s="9"/>
     </row>
     <row r="44" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
@@ -6348,18 +6349,18 @@
       <c r="AK44" s="20"/>
       <c r="AL44" s="20"/>
       <c r="AM44" s="20"/>
-      <c r="AN44" s="20"/>
-      <c r="AO44" s="20"/>
-      <c r="AP44" s="20"/>
-      <c r="AQ44" s="20"/>
-      <c r="AR44" s="20"/>
-      <c r="AS44" s="20"/>
-      <c r="AT44" s="20"/>
-      <c r="AU44" s="28"/>
-      <c r="AV44" s="28"/>
-      <c r="AW44" s="28"/>
-      <c r="AX44" s="28"/>
-      <c r="AY44" s="28"/>
+      <c r="AN44" s="9"/>
+      <c r="AO44" s="9"/>
+      <c r="AP44" s="9"/>
+      <c r="AQ44" s="9"/>
+      <c r="AR44" s="9"/>
+      <c r="AS44" s="9"/>
+      <c r="AT44" s="9"/>
+      <c r="AU44" s="9"/>
+      <c r="AV44" s="9"/>
+      <c r="AW44" s="9"/>
+      <c r="AX44" s="9"/>
+      <c r="AY44" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>